<commit_message>
updated BOM and pick and place
</commit_message>
<xml_diff>
--- a/Schematics/sensor_hub_BOM_JLCPCB.xlsx
+++ b/Schematics/sensor_hub_BOM_JLCPCB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\Auto-Water-Base\Schematics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cools\Documents\Repositories\Senior Design\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75833A6-ABB0-4F44-A7E5-80E1CF411E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E1CFFB-CBB2-44F9-9A5D-1197883C660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{4C850F2F-DC45-403E-95F1-25BAB81A96F3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4C850F2F-DC45-403E-95F1-25BAB81A96F3}"/>
   </bookViews>
   <sheets>
     <sheet name="JLCPCB_BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="120">
   <si>
     <t>Comment</t>
   </si>
@@ -306,6 +306,96 @@
   </si>
   <si>
     <t>Crystal:Crystal_SMD_3215-2Pin_3.2x1.5mm</t>
+  </si>
+  <si>
+    <t>C967766</t>
+  </si>
+  <si>
+    <t>C3013946</t>
+  </si>
+  <si>
+    <t>C54313</t>
+  </si>
+  <si>
+    <t>C116352</t>
+  </si>
+  <si>
+    <t>C1779</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>C1711</t>
+  </si>
+  <si>
+    <t>C63339</t>
+  </si>
+  <si>
+    <t>C45783</t>
+  </si>
+  <si>
+    <t>C46653</t>
+  </si>
+  <si>
+    <t>C111566</t>
+  </si>
+  <si>
+    <t>C2297</t>
+  </si>
+  <si>
+    <t>C779674</t>
+  </si>
+  <si>
+    <t>C79382</t>
+  </si>
+  <si>
+    <t>C165948</t>
+  </si>
+  <si>
+    <t>C131339</t>
+  </si>
+  <si>
+    <t>C22438292</t>
+  </si>
+  <si>
+    <t>C154797</t>
+  </si>
+  <si>
+    <t>C218607</t>
+  </si>
+  <si>
+    <t>C2077400</t>
+  </si>
+  <si>
+    <t>C322246</t>
+  </si>
+  <si>
+    <t>C26023</t>
+  </si>
+  <si>
+    <t>C126687</t>
+  </si>
+  <si>
+    <t>C2828726</t>
+  </si>
+  <si>
+    <t>C25275</t>
+  </si>
+  <si>
+    <t>C17414</t>
+  </si>
+  <si>
+    <t>C17552</t>
+  </si>
+  <si>
+    <t>C26011</t>
+  </si>
+  <si>
+    <t>C25623</t>
+  </si>
+  <si>
+    <t>C86781</t>
   </si>
 </sst>
 </file>
@@ -762,16 +852,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145F5FD1-34DB-4C68-82A4-37DC1C7F42E0}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="24.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.3828125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.61328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -799,7 +889,9 @@
       <c r="C2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="10" t="s">
@@ -811,7 +903,9 @@
       <c r="C3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
@@ -823,7 +917,9 @@
       <c r="C4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="10" t="s">
@@ -835,7 +931,9 @@
       <c r="C5" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
@@ -847,7 +945,9 @@
       <c r="C6" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
@@ -859,7 +959,9 @@
       <c r="C7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
@@ -871,7 +973,9 @@
       <c r="C8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="10" t="s">
@@ -883,7 +987,9 @@
       <c r="C9" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="10" t="s">
@@ -895,7 +1001,9 @@
       <c r="C10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="10" t="s">
@@ -907,7 +1015,9 @@
       <c r="C11" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="10" t="s">
@@ -919,7 +1029,9 @@
       <c r="C12" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="10" t="s">
@@ -943,7 +1055,9 @@
       <c r="C14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="10" t="s">
@@ -955,7 +1069,9 @@
       <c r="C15" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="10" t="s">
@@ -967,7 +1083,9 @@
       <c r="C16" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
@@ -979,7 +1097,9 @@
       <c r="C17" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="10" t="s">
@@ -991,7 +1111,9 @@
       <c r="C18" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="10" t="s">
@@ -1003,7 +1125,9 @@
       <c r="C19" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="10" t="s">
@@ -1015,7 +1139,9 @@
       <c r="C20" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10" t="s">
@@ -1027,7 +1153,9 @@
       <c r="C21" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="10" t="s">
@@ -1039,7 +1167,9 @@
       <c r="C22" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="10">
@@ -1051,7 +1181,9 @@
       <c r="C23" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="10" t="s">
@@ -1063,7 +1195,9 @@
       <c r="C24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="10" t="s">
@@ -1077,7 +1211,7 @@
       </c>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="27.45">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" s="10" t="s">
         <v>63</v>
       </c>
@@ -1087,7 +1221,9 @@
       <c r="C26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="10">
@@ -1099,7 +1235,9 @@
       <c r="C27" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="10" t="s">
@@ -1111,7 +1249,9 @@
       <c r="C28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="10" t="s">
@@ -1123,7 +1263,9 @@
       <c r="C29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="10" t="s">
@@ -1135,7 +1277,9 @@
       <c r="C30" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="10" t="s">
@@ -1147,7 +1291,9 @@
       <c r="C31" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="10" t="s">
@@ -1171,7 +1317,9 @@
       <c r="C33" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="10" t="s">
@@ -1183,7 +1331,9 @@
       <c r="C34" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="10" t="s">
@@ -1195,7 +1345,9 @@
       <c r="C35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="10" t="s">
@@ -1207,7 +1359,9 @@
       <c r="C36" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="10" t="s">
@@ -1238,6 +1392,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>